<commit_message>
Update Meteora Ecommerce - FINAL AULA 1.xlsx
</commit_message>
<xml_diff>
--- a/Excel/Basico/Curso 01/Meteora Ecommerce - FINAL AULA 1.xlsx
+++ b/Excel/Basico/Curso 01/Meteora Ecommerce - FINAL AULA 1.xlsx
@@ -1,42 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://officeresolve-my.sharepoint.com/personal/r_sabino_officeresolve_com_br/Documents/Alura-Ciência de Dados/03.01 - Novas Formações Excel/Formação Excel/3195 - Excel 1 - Domine o Editor de planilhas/Materiais do Curso/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\exercicios\alura\Excel\Basico\Curso 01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="143" documentId="8_{0D071335-E186-43B8-A2BC-FF91FCFBAFB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{653020B6-5AB9-4AB9-9CCB-FC0BB8A301C6}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4CEC536-0093-4152-93A0-2AA2EF2A4EDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="20640" windowHeight="11040" xr2:uid="{F6D97A53-F63B-4272-A181-44B26E0B790F}"/>
+    <workbookView xWindow="28692" yWindow="624" windowWidth="19416" windowHeight="11496" activeTab="1" xr2:uid="{F6D97A53-F63B-4272-A181-44B26E0B790F}"/>
   </bookViews>
   <sheets>
-    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="Produtos" sheetId="1" r:id="rId1"/>
+    <sheet name="Tabela de Produtos" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="24">
   <si>
     <t>Produtos</t>
   </si>
@@ -99,13 +89,25 @@
   </si>
   <si>
     <t>Calçado</t>
+  </si>
+  <si>
+    <t>Meteora</t>
+  </si>
+  <si>
+    <t>Coluna1</t>
+  </si>
+  <si>
+    <t>Quantidade</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <numFmts count="1">
+    <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -121,13 +123,76 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="9" tint="-0.499984740745262"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDAFF01"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -139,23 +204,318 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Moeda" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="15">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill patternType="darkVertical">
+          <fgColor theme="4"/>
+          <bgColor theme="1" tint="0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="Estilo 1" pivot="0" count="1" xr9:uid="{12128D1B-C159-4085-B510-D5D9EBDB8E8E}">
+      <tableStyleElement type="firstRowStripe" dxfId="14"/>
+    </tableStyle>
+  </tableStyles>
+  <colors>
+    <mruColors>
+      <color rgb="FFDAFF01"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -165,6 +525,21 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D6754171-352E-4C2C-841A-E71FA758B516}" name="Tabela1" displayName="Tabela1" ref="A3:F24" totalsRowCount="1" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="A3:F23" xr:uid="{D6754171-352E-4C2C-841A-E71FA758B516}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{837A74C9-646E-44B5-8F62-ACD0EEBD4E45}" name="Produtos" dataDxfId="13" totalsRowDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{9F33F732-466B-49B5-BC95-381F16062427}" name="Tamanho" dataDxfId="12" totalsRowDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{32B3D5A2-20D3-41E3-9C6F-19FF001589F8}" name="Categoria" dataDxfId="11" totalsRowDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{B5B53EE7-8082-45FD-A399-60FE201CFCFC}" name="Quantidade" dataDxfId="7" totalsRowDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{7E2DC10D-F33F-4816-874B-5BE5DA6CD0A5}" name="Preço Unitário" dataDxfId="10" totalsRowDxfId="1" dataCellStyle="Moeda"/>
+    <tableColumn id="6" xr3:uid="{3A329CE6-5CA3-4E03-BA59-92937B2979C6}" name="Coluna1" dataDxfId="6" totalsRowDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -466,309 +841,309 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7162DC3F-8DD7-4F1A-A109-A490D58F15DD}">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.88671875" customWidth="1"/>
-    <col min="2" max="2" width="11.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.88671875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.88671875" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:4" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2">
+      <c r="C2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="3">
         <v>25.9</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3">
+      <c r="C3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="3">
         <v>29.9</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4">
+      <c r="C4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="3">
         <v>32.9</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="3">
         <v>399.9</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6">
+      <c r="C6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="3">
         <v>249.9</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7">
+      <c r="C7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="3">
         <v>259.89999999999998</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C8" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8">
+      <c r="C8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="3">
         <v>299.89999999999998</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9">
+      <c r="C9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="3">
         <v>85.9</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10">
+      <c r="C10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="3">
         <v>89.9</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="A11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11">
+      <c r="C11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="3">
         <v>92.9</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="A12" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12">
+      <c r="C12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="3">
         <v>149.9</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="A13" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C13" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13">
+      <c r="C13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="3">
         <v>65.900000000000006</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="A14" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C14" t="s">
-        <v>18</v>
-      </c>
-      <c r="D14">
+      <c r="C14" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="3">
         <v>69.900000000000006</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="A15" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C15" t="s">
-        <v>18</v>
-      </c>
-      <c r="D15">
+      <c r="C15" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="3">
         <v>70.900000000000006</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="A16" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16" s="2">
         <v>36</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="3">
         <v>199.9</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="A17" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B17" s="2">
         <v>37</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="3">
         <v>249.9</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="A18" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B18" s="2">
         <v>38</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="3">
         <v>259.89999999999998</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+      <c r="A19" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="3">
         <v>259.89999999999998</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+      <c r="A20" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="3">
         <v>39.9</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+      <c r="A21" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="3">
         <v>49.9</v>
       </c>
     </row>
@@ -776,4 +1151,437 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A8C14DC-A92E-433E-A1C0-54B066722618}">
+  <dimension ref="A1:F24"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.109375" style="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19" style="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.109375" style="16" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="A1" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+    </row>
+    <row r="2" spans="1:6" ht="1.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="7"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="9"/>
+    </row>
+    <row r="3" spans="1:6" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A3" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="12">
+        <v>4</v>
+      </c>
+      <c r="E4" s="13">
+        <v>5</v>
+      </c>
+      <c r="F4" s="17"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="12">
+        <v>5</v>
+      </c>
+      <c r="E5" s="13">
+        <v>29.9</v>
+      </c>
+      <c r="F5" s="12"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="12">
+        <v>9</v>
+      </c>
+      <c r="E6" s="13">
+        <v>32.9</v>
+      </c>
+      <c r="F6" s="12"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="12">
+        <v>9</v>
+      </c>
+      <c r="E7" s="13">
+        <v>399.9</v>
+      </c>
+      <c r="F7" s="12"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="12">
+        <v>4</v>
+      </c>
+      <c r="E8" s="13">
+        <v>249.9</v>
+      </c>
+      <c r="F8" s="12"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="12">
+        <v>2</v>
+      </c>
+      <c r="E9" s="13">
+        <v>259.89999999999998</v>
+      </c>
+      <c r="F9" s="12"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="12">
+        <v>5</v>
+      </c>
+      <c r="E10" s="13">
+        <v>299.89999999999998</v>
+      </c>
+      <c r="F10" s="12"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="12">
+        <v>10</v>
+      </c>
+      <c r="E11" s="13">
+        <v>85.9</v>
+      </c>
+      <c r="F11" s="12"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="12">
+        <v>20</v>
+      </c>
+      <c r="E12" s="13">
+        <v>89.9</v>
+      </c>
+      <c r="F12" s="12"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="12">
+        <v>2</v>
+      </c>
+      <c r="E13" s="13">
+        <v>92.9</v>
+      </c>
+      <c r="F13" s="12"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="12">
+        <v>1</v>
+      </c>
+      <c r="E14" s="13">
+        <v>149.9</v>
+      </c>
+      <c r="F14" s="12"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="12">
+        <v>5</v>
+      </c>
+      <c r="E15" s="13">
+        <v>65.900000000000006</v>
+      </c>
+      <c r="F15" s="12"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="12">
+        <v>4</v>
+      </c>
+      <c r="E16" s="13">
+        <v>69.900000000000006</v>
+      </c>
+      <c r="F16" s="12"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="12">
+        <v>6</v>
+      </c>
+      <c r="E17" s="13">
+        <v>70.900000000000006</v>
+      </c>
+      <c r="F17" s="12"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" s="12">
+        <v>36</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D18" s="12">
+        <v>7</v>
+      </c>
+      <c r="E18" s="13">
+        <v>199.9</v>
+      </c>
+      <c r="F18" s="12"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" s="12">
+        <v>37</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D19" s="12">
+        <v>8</v>
+      </c>
+      <c r="E19" s="13">
+        <v>249.9</v>
+      </c>
+      <c r="F19" s="12"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" s="12">
+        <v>38</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D20" s="12">
+        <v>9</v>
+      </c>
+      <c r="E20" s="13">
+        <v>259.89999999999998</v>
+      </c>
+      <c r="F20" s="12"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21" s="12">
+        <v>1</v>
+      </c>
+      <c r="E21" s="13">
+        <v>259.89999999999998</v>
+      </c>
+      <c r="F21" s="12"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D22" s="12">
+        <v>10</v>
+      </c>
+      <c r="E22" s="13">
+        <v>39.9</v>
+      </c>
+      <c r="F22" s="12"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D23" s="12">
+        <v>5</v>
+      </c>
+      <c r="E23" s="13">
+        <v>49.9</v>
+      </c>
+      <c r="F23" s="12"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="12"/>
+      <c r="B24" s="12"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="12"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>